<commit_message>
Updates to get dispatch and vehicle shares working
</commit_message>
<xml_diff>
--- a/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
+++ b/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/users/nathaniyer/library/containers/com.microsoft.excel/data/state-eps-data-repository/template_state/elec/bgdpbes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\California\Models\eps-california\InputData\elec\BGDPbES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094B831B-97A2-1F47-B0E7-C814EF427FC9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FD48E3-F2AB-4F32-8B73-FA4805E16796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="460" windowWidth="23000" windowHeight="11060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -503,11 +503,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -515,42 +515,42 @@
         <v>44307</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -568,15 +568,17 @@
   </sheetPr>
   <dimension ref="A1:AK17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:37" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
@@ -689,7 +691,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -837,7 +839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -985,7 +987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1133,7 +1135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1281,599 +1283,599 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ9">
         <f t="shared" ref="D9:AK14" si="2">$B9</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -2021,7 +2023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -2169,7 +2171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -2317,7 +2319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -2465,155 +2467,155 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14">
         <f>$B14</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -2726,7 +2728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -2839,7 +2841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
Updates to power sector for curtailment and moving CHP out of flexible resources; updates to fuel balancing priorities
</commit_message>
<xml_diff>
--- a/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
+++ b/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\California\Models\eps-california\InputData\elec\BGDPbES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\California\Models\eps-california\InputData\elec\BGDPbES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2EBF83-380A-4DB6-AE01-A7BC70F86767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0376537F-F115-4CAB-A708-3D1238042804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -569,7 +569,7 @@
   <dimension ref="A1:AK17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B15" sqref="B15:AK15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2620,112 +2620,112 @@
         <v>22</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updates moving in front of the meter cogeneration out of the industry sector and into the power sector; CHP plants are no long tracked separately and are included with natural gas nonpeaker preexisting nonretiring
</commit_message>
<xml_diff>
--- a/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
+++ b/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\California\Models\eps-california\InputData\elec\BGDPbES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0376537F-F115-4CAB-A708-3D1238042804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13BB2B9F-50DC-430A-A1A3-017C65232250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2620,112 +2620,112 @@
         <v>22</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated mdl, bgdpbes, mppc, brspbs, tts
</commit_message>
<xml_diff>
--- a/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
+++ b/InputData/elec/BGDPbES/BAU Guaranteed Dispatch Perc by Elec Source.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olivia Ashmoore\Documents\EPS_Models by Region\RMI\RMI_all_states\CA\elec\BGDPbES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7CF3399D-9D11-46BD-96FC-E6234C4D6952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4DA8A2D0-2E29-4054-AB40-04B01813D86D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13395" yWindow="345" windowWidth="15360" windowHeight="16755" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="12330" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -618,7 +618,7 @@
         <v>60</v>
       </c>
       <c r="C1" s="7">
-        <v>45236</v>
+        <v>45265</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2493,7 +2493,7 @@
   <dimension ref="A1:AK25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:AK22"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2793,7 +2793,7 @@
         <v>0</v>
       </c>
       <c r="S3">
-        <f t="shared" ref="J3:AK10" si="1">$B3</f>
+        <f t="shared" ref="J3:AK9" si="1">$B3</f>
         <v>0</v>
       </c>
       <c r="T3">
@@ -3719,140 +3719,112 @@
         <v>5</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI10">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ10">
-        <f t="shared" ref="G10:AK15" si="2">$B10</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK10">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
@@ -3860,138 +3832,112 @@
         <v>7</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK11">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.25">
@@ -4003,143 +3949,143 @@
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="C12">
-        <f t="shared" ref="C12:I12" si="3">$B12</f>
+        <f t="shared" ref="C12:I12" si="2">$B12</f>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="D12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="E12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="F12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="G12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="H12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="I12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="J12">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="G12:AK15" si="3">$B12</f>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="K12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="L12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="M12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="N12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="O12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="P12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="R12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="S12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="T12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="U12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="V12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="W12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="X12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="Y12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="Z12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="AA12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="AB12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="AC12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="AD12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="AE12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="AF12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="AG12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="AH12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="AI12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="AJ12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
       <c r="AK12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6003999999999998E-2</v>
       </c>
     </row>
@@ -4163,127 +4109,127 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="V13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="X13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Y13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Z13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AA13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AB13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AD13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AE13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AG13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AH13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AI13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AJ13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AK13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -4316,115 +4262,115 @@
         <v>0</v>
       </c>
       <c r="J14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="V14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="X14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Y14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Z14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AA14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AB14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AD14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AE14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AG14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AH14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AI14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AJ14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AK14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -4460,111 +4406,111 @@
         <v>0</v>
       </c>
       <c r="K15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="V15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="X15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Y15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Z15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AA15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AB15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AD15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AE15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AF15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AG15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AH15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AI15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AJ15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AK15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>